<commit_message>
Initializing footer buttons component
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\SN\projectui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snh\Documents\Gestion du Budget\dev\gesbudgetui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{291AEA75-17BE-43CC-B35B-B7B3FCC9CA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1770" windowWidth="14400" windowHeight="7370" xr2:uid="{AF263832-F7EC-43C8-B67C-76F924366205}"/>
+    <workbookView xWindow="3615" yWindow="1770" windowWidth="14400" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>etat == INIT</t>
   </si>
@@ -118,12 +117,33 @@
   </si>
   <si>
     <t>isbtnOptionsAnnuler</t>
+  </si>
+  <si>
+    <t>statut == VALIDS</t>
+  </si>
+  <si>
+    <t>! currentUserValidS</t>
+  </si>
+  <si>
+    <t>hasPermission (VALIDF)</t>
+  </si>
+  <si>
+    <t>! hasPermission (VALIDF)</t>
+  </si>
+  <si>
+    <t>currentUserValidS</t>
+  </si>
+  <si>
+    <t>superior validated</t>
+  </si>
+  <si>
+    <t>statut == VALIDF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,10 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,290 +501,395 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7267B8-8A4D-487D-ACEA-B027D74D8394}">
-  <dimension ref="A1:G54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F7" s="1" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F21" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F22" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F23" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F25" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F26" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D29" t="s">
+    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G33" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="F41" t="s">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="F42" t="s">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="F44" t="s">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="F45" t="s">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="F46" t="s">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E49" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E50" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E52" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E53" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E54" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>37</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing footerbuttons to re-render when entity Props change
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snh\Documents\Gestion du Budget\dev\gesbudgetui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\SN\projectui\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3134E9D4-0EF5-485C-9B80-0D1D6C04FDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="1770" windowWidth="14400" windowHeight="7365"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>etat == INIT</t>
   </si>
@@ -138,12 +139,15 @@
   </si>
   <si>
     <t>statut == VALIDF</t>
+  </si>
+  <si>
+    <t>No superior validated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -177,17 +181,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,394 +596,545 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="6"/>
+      <c r="E16" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="6"/>
+      <c r="E17" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="6"/>
+      <c r="E18" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="6"/>
+      <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="6"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
+    <row r="22" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
+    <row r="23" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+    <row r="24" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="6"/>
+      <c r="E24" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="1" t="s">
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
+    <row r="26" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D28" s="9"/>
+      <c r="E28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D29" s="9"/>
+      <c r="E29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="D29" s="3" t="s">
+    <row r="42" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="D42" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E43" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="1" t="s">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E44" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="1" t="s">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="G46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="1" t="s">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E48" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="E49" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="1" t="s">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G51" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="E53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="1" t="s">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="1" t="s">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F55" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F44" s="1" t="s">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F57" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F45" s="1" t="s">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F58" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F46" s="1" t="s">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E49" s="1" t="s">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="E62" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E50" s="1" t="s">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="E63" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D64" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="1" t="s">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E65" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E53" s="1" t="s">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E66" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E67" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D70" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E58" s="1" t="s">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E71" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E59" s="1" t="s">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E72" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F60" t="s">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F73" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="1" t="s">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G74" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D75" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E63" s="1" t="s">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E76" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E64" s="1" t="s">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D79" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="1" t="s">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E80" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="1" t="s">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E81" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D82" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="1" t="s">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E83" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="1" t="s">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E84" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E85" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
         <v>37</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initializing new logic for footerbuttons
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\SN\projectui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snh\Documents\Gestion du Budget\dev\gesbudgetui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3134E9D4-0EF5-485C-9B80-0D1D6C04FDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="46">
   <si>
     <t>etat == INIT</t>
   </si>
@@ -142,12 +142,33 @@
   </si>
   <si>
     <t>No superior validated</t>
+  </si>
+  <si>
+    <t>hasPermission(VALIDP) &amp;&amp; next_statut == null</t>
+  </si>
+  <si>
+    <t>superior Validated F</t>
+  </si>
+  <si>
+    <t>No superior validated F</t>
+  </si>
+  <si>
+    <t>isbtnValiderP</t>
+  </si>
+  <si>
+    <t>hasPermission (VALIDF) &amp;&amp; next_statut == null</t>
+  </si>
+  <si>
+    <t>hasPermission (IMPUTER)</t>
+  </si>
+  <si>
+    <t>isbtnImputer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,12 +186,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -265,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,6 +310,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,179 +628,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B86" sqref="B86:C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D16" s="6"/>
       <c r="E16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D17" s="6"/>
       <c r="E17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D18" s="6"/>
       <c r="E18" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D20" s="6"/>
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D21" s="6"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D22" s="6"/>
       <c r="E22" s="9"/>
       <c r="F22" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D23" s="6"/>
       <c r="E23" s="9"/>
       <c r="F23" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D24" s="6"/>
       <c r="E24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D25" s="6"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="4:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27" s="9" t="s">
         <v>29</v>
       </c>
@@ -778,7 +810,7 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" s="9"/>
       <c r="E28" s="14" t="s">
         <v>14</v>
@@ -788,7 +820,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29" s="9"/>
       <c r="E29" s="14" t="s">
         <v>18</v>
@@ -798,7 +830,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="9" t="s">
         <v>38</v>
       </c>
@@ -808,7 +840,7 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
         <v>5</v>
@@ -818,7 +850,7 @@
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="14" t="s">
@@ -828,7 +860,7 @@
       <c r="H32" s="9"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="14" t="s">
@@ -838,7 +870,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="14" t="s">
@@ -848,7 +880,7 @@
       <c r="H34" s="9"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D35" s="9"/>
       <c r="E35" s="9" t="s">
         <v>12</v>
@@ -858,7 +890,7 @@
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="14" t="s">
@@ -868,7 +900,7 @@
       <c r="H36" s="9"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="14" t="s">
@@ -878,7 +910,7 @@
       <c r="H37" s="9"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="14" t="s">
@@ -888,254 +920,1447 @@
       <c r="H38" s="9"/>
       <c r="I38" s="14"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E48" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E49" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G51" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F55" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F57" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F58" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E62" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E63" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E65" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E66" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E67" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E71" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E72" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G74" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E76" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E80" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E83" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E84" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E85" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="9"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="K27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="L29" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="8"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="19"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="8"/>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="I41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="8"/>
+    </row>
+    <row r="42" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="K42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="8"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="L43" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N43" s="8"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="M44" t="s">
+        <v>5</v>
+      </c>
+      <c r="N44" s="8"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="N45" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" t="s">
+        <v>25</v>
+      </c>
+      <c r="N46" s="8"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="L47" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" s="8"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="M48" t="s">
+        <v>5</v>
+      </c>
+      <c r="N48" s="8"/>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="N49" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="K50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G51" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="M52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="N53" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="N54" s="8"/>
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="N55" s="8"/>
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="N56" s="8"/>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="N57" s="8"/>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="N58" s="8"/>
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="N59" s="8"/>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="J60" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" s="8"/>
+    </row>
+    <row r="61" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="K61" t="s">
+        <v>29</v>
+      </c>
+      <c r="N61" s="8"/>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="L62" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N62" s="8"/>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="L63" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N63" s="8"/>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="K64" t="s">
+        <v>16</v>
+      </c>
+      <c r="N64" s="8"/>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="L65" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N65" s="8"/>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="8"/>
+      <c r="N66" s="8"/>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="8"/>
+      <c r="N67" s="8"/>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="8"/>
+      <c r="I68" t="s">
+        <v>31</v>
+      </c>
+      <c r="N68" s="8"/>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="I69" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J69" t="s">
+        <v>32</v>
+      </c>
+      <c r="K69" t="s">
+        <v>43</v>
+      </c>
+      <c r="N69" s="8"/>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" s="8"/>
+      <c r="L70" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N70" s="8"/>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="L71" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N71" s="8"/>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="K72" t="s">
+        <v>27</v>
+      </c>
+      <c r="N72" s="8"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" s="8"/>
+      <c r="L73" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N73" s="8"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G74" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" s="8"/>
+      <c r="N75" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="8"/>
+      <c r="N76" s="8"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" s="8"/>
+      <c r="N77" s="8"/>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="8"/>
+      <c r="J78" t="s">
+        <v>35</v>
+      </c>
+      <c r="N78" s="8"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" s="8"/>
+      <c r="K79" t="s">
+        <v>36</v>
+      </c>
+      <c r="N79" s="8"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80" s="8"/>
+      <c r="L80" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N80" s="8"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="8"/>
+      <c r="L81" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N81" s="8"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G82" s="8"/>
+      <c r="K82" t="s">
+        <v>16</v>
+      </c>
+      <c r="N82" s="8"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="8"/>
+      <c r="L83" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N83" s="8"/>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G84" s="8"/>
+      <c r="N84" s="8"/>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="8"/>
+      <c r="N85" s="8"/>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>37</v>
+      </c>
+      <c r="G86" s="8"/>
+      <c r="I86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>6</v>
+      </c>
+      <c r="G87" s="8"/>
+      <c r="I87" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" s="8"/>
+      <c r="I88" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G89" s="8"/>
+      <c r="K89" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L90" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>